<commit_message>
code updated to fix parallel test
</commit_message>
<xml_diff>
--- a/Data/WeatherData.xlsx
+++ b/Data/WeatherData.xlsx
@@ -24,22 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
-  <si>
-    <t>Method</t>
-  </si>
-  <si>
-    <t>Endpoint</t>
-  </si>
-  <si>
-    <t>Lat</t>
-  </si>
-  <si>
-    <t>Lon</t>
-  </si>
-  <si>
-    <t>API_Key</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
   <si>
     <t>GET</t>
   </si>
@@ -50,9 +35,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>BaseURL</t>
-  </si>
-  <si>
     <t>http://api.openweathermap.org</t>
   </si>
   <si>
@@ -63,12 +45,6 @@
   </si>
   <si>
     <t>-71.0589</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>HTTPStatus</t>
   </si>
   <si>
     <t>/data/2.6/weather?</t>
@@ -395,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,74 +392,74 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
+      <c r="E1" s="1">
+        <v>42.360100000000003</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
         <v>42.360100000000003</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H2" s="1">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1">
-        <v>42.360100000000003</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
       </c>
       <c r="H3" s="1">
         <v>400</v>
@@ -491,102 +467,76 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42.360100000000003</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
       <c r="H4" s="1">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>42.360100000000003</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H5" s="1">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1">
         <v>42.360100000000003</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H6" s="1">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1">
-        <v>42.360100000000003</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="1">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
proper error messages are logged to logs
</commit_message>
<xml_diff>
--- a/Data/WeatherData.xlsx
+++ b/Data/WeatherData.xlsx
@@ -398,7 +398,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +460,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="1">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>